<commit_message>
Updated with new blog content
</commit_message>
<xml_diff>
--- a/WorkLifeBalance_Share.xlsx
+++ b/WorkLifeBalance_Share.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Apps\MarkdownPro\WorkLifeBalance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\GitHub\WorkLifeBalance\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E2716D-1F3A-456E-935B-2A9D0BECC39C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27120" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WorkLifeBalance" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="Slicer_Expectation">#N/A</definedName>
     <definedName name="Slicer_Expectation1">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -30,12 +31,21 @@
         <x14:slicerCache r:id="rId4"/>
       </x15:slicerCaches>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>Expectation</t>
   </si>
@@ -111,11 +121,14 @@
   <si>
     <t>** Clear any filter in the Slicer.   Enter values in Yellow area.  Each month should total 100</t>
   </si>
+  <si>
+    <t>Enter values:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -669,13 +682,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2218,6 +2231,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B8E1-4120-AA7D-ED7FBA898C60}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2237,6 +2255,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B8E1-4120-AA7D-ED7FBA898C60}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -7832,8 +7855,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>154680</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="Expectation">
@@ -7856,7 +7879,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8029,8 +8052,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>16283</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Expectation 1">
@@ -8053,7 +8076,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8098,7 +8121,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Expectation" sourceName="Expectation">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Expectation" xr10:uid="{00000000-0013-0000-FFFF-FFFF01000000}" sourceName="Expectation">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="2" column="1"/>
@@ -8108,7 +8131,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Expectation1" sourceName="Expectation">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Expectation1" xr10:uid="{00000000-0013-0000-FFFF-FFFF02000000}" sourceName="Expectation">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="4" column="1"/>
@@ -8118,44 +8141,44 @@
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Expectation" cache="Slicer_Expectation" caption="Expectation" rowHeight="241300"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Expectation" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="Slicer_Expectation" caption="Expectation" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Expectation 1" cache="Slicer_Expectation1" caption="Expectation" rowHeight="241300"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Expectation 1" xr10:uid="{00000000-0014-0000-FFFF-FFFF02000000}" cache="Slicer_Expectation1" caption="Expectation" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Results" displayName="Results" ref="B16:N21" totalsRowShown="0">
-  <autoFilter ref="B16:N21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Results" displayName="Results" ref="B16:N21" totalsRowShown="0">
+  <autoFilter ref="B16:N21" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Expectation"/>
-    <tableColumn id="2" name="Jan"/>
-    <tableColumn id="3" name="Feb"/>
-    <tableColumn id="4" name="Mar"/>
-    <tableColumn id="5" name="Apr"/>
-    <tableColumn id="6" name="May"/>
-    <tableColumn id="7" name="Jun"/>
-    <tableColumn id="8" name="Jul"/>
-    <tableColumn id="9" name="Aug"/>
-    <tableColumn id="10" name="Sep"/>
-    <tableColumn id="11" name="Oct"/>
-    <tableColumn id="12" name="Nov"/>
-    <tableColumn id="13" name="Dec"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Expectation"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Jan"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Feb"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Mar"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Apr"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="May"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Jun"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Jul"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Aug"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Sep"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Oct"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Nov"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Dec"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="BalancePCT" displayName="BalancePCT" ref="S16:T18" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="BalancePCT" displayName="BalancePCT" ref="S16:T18" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Classification"/>
-    <tableColumn id="2" name="Value">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Classification"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Value">
       <calculatedColumnFormula>SUMIF(P16:Q20,S17,Q16:Q20)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8164,32 +8187,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Results5" displayName="Results5" ref="B16:N21" totalsRowShown="0">
-  <autoFilter ref="B16:N21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Results5" displayName="Results5" ref="B16:N21" totalsRowShown="0">
+  <autoFilter ref="B16:N21" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Expectation"/>
-    <tableColumn id="2" name="Jan" dataDxfId="11"/>
-    <tableColumn id="3" name="Feb" dataDxfId="10"/>
-    <tableColumn id="4" name="Mar" dataDxfId="9"/>
-    <tableColumn id="5" name="Apr" dataDxfId="8"/>
-    <tableColumn id="6" name="May" dataDxfId="7"/>
-    <tableColumn id="7" name="Jun" dataDxfId="6"/>
-    <tableColumn id="8" name="Jul" dataDxfId="5"/>
-    <tableColumn id="9" name="Aug" dataDxfId="4"/>
-    <tableColumn id="10" name="Sep" dataDxfId="3"/>
-    <tableColumn id="11" name="Oct" dataDxfId="2"/>
-    <tableColumn id="12" name="Nov" dataDxfId="1"/>
-    <tableColumn id="13" name="Dec" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Expectation"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Jan" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Feb" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Mar" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Apr" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="May" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Jun" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Jul" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Aug" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Sep" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Oct" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Nov" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Dec" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="BalancePCT6" displayName="BalancePCT6" ref="S16:T18" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="BalancePCT6" displayName="BalancePCT6" ref="S16:T18" totalsRowShown="0">
   <tableColumns count="2">
-    <tableColumn id="1" name="Classification"/>
-    <tableColumn id="2" name="Value">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Classification"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Value">
       <calculatedColumnFormula>SUMIF(P16:Q20,S17,Q16:Q20)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8493,11 +8516,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8534,21 +8557,21 @@
       <c r="T1" s="9"/>
     </row>
     <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -8922,6 +8945,11 @@
       <c r="Q23" s="4">
         <f>SUM(Q17:Q22)</f>
         <v>1200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -8947,7 +8975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
@@ -8988,21 +9016,21 @@
       <c r="T1" s="9"/>
     </row>
     <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -9061,40 +9089,40 @@
       <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <v>20</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="8">
         <v>20</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="8">
         <v>20</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="8">
         <v>20</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="8">
         <v>20</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="8">
         <v>20</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>20</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="8">
         <v>20</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="8">
         <v>20</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="8">
         <v>20</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="8">
         <v>20</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="8">
         <v>20</v>
       </c>
       <c r="P17" s="4" t="s">
@@ -9116,40 +9144,40 @@
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>20</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="8">
         <v>20</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <v>20</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="8">
         <v>20</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="8">
         <v>20</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="8">
         <v>20</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="8">
         <v>20</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="8">
         <v>20</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="8">
         <v>20</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="8">
         <v>20</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="8">
         <v>20</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="8">
         <v>20</v>
       </c>
       <c r="P18" s="5" t="s">
@@ -9171,40 +9199,40 @@
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>20</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>20</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>20</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="8">
         <v>20</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="8">
         <v>20</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="8">
         <v>20</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="8">
         <v>20</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="8">
         <v>20</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="8">
         <v>20</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="8">
         <v>20</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="8">
         <v>20</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="8">
         <v>20</v>
       </c>
       <c r="P19" s="4" t="s">
@@ -9226,40 +9254,40 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>20</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="8">
         <v>20</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="8">
         <v>20</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="8">
         <v>20</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="8">
         <v>20</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="8">
         <v>20</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="8">
         <v>20</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="8">
         <v>20</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="8">
         <v>20</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="8">
         <v>20</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="8">
         <v>20</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="8">
         <v>20</v>
       </c>
       <c r="P20" s="5" t="s">
@@ -9274,40 +9302,40 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>20</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="8">
         <v>20</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="8">
         <v>20</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="8">
         <v>20</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="8">
         <v>20</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="8">
         <v>20</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="8">
         <v>20</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="8">
         <v>20</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="8">
         <v>20</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="8">
         <v>20</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="8">
         <v>20</v>
       </c>
-      <c r="N21" s="10">
+      <c r="N21" s="8">
         <v>20</v>
       </c>
       <c r="P21" s="4" t="s">

</xml_diff>